<commit_message>
fix Industrial sheet formula
</commit_message>
<xml_diff>
--- a/summary_statistics/SUMMARY_NATIONAL_2020-2050.xlsx
+++ b/summary_statistics/SUMMARY_NATIONAL_2020-2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/npaul/GEM/africa-exposure-data/summary_statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDC7653-1CE7-5B4D-9D1C-DEB9EBF5246E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9684A1-4DEE-CC4B-9E8B-570C898372E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="460" windowWidth="19080" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9240" yWindow="460" windowWidth="19080" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOTAL" sheetId="1" r:id="rId1"/>
@@ -1250,7 +1250,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2398,8 +2398,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:AJ56" totalsRowShown="0">
   <autoFilter ref="A2:AJ56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AJ773">
-    <sortCondition ref="B2:B773"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AJ56">
+    <sortCondition ref="B2:B56"/>
   </sortState>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="REGION"/>
@@ -2546,8 +2546,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ADD439DB-F4E8-FB43-9385-7CC5B6A99A86}" name="Table1345" displayName="Table1345" ref="A2:T56" totalsRowShown="0">
   <autoFilter ref="A2:T56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:T773">
-    <sortCondition ref="B2:B773"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:T56">
+    <sortCondition ref="B2:B56"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{891F41A9-EA27-5A47-BCD1-C45C51EE677A}" name="REGION"/>
@@ -2569,10 +2569,10 @@
     <tableColumn id="29" xr3:uid="{B00E6E66-2041-B640-97FA-5128B536C5A4}" name="2045_TOTAL_REPL_COST_USD" dataDxfId="3" dataCellStyle="Comma"/>
     <tableColumn id="31" xr3:uid="{FE5704CB-4534-2540-9A6E-569BB8757CBA}" name="2050_TOTAL_REPL_COST_USD" dataDxfId="2" dataCellStyle="Comma"/>
     <tableColumn id="32" xr3:uid="{3AA7F3FC-2991-A441-BF40-8493B5BF4480}" name="INCR_BUILDINGS" dataDxfId="1" dataCellStyle="Percent">
-      <calculatedColumnFormula>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</calculatedColumnFormula>
+      <calculatedColumnFormula>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{3699C7A8-5BF2-9243-878D-770081D4324A}" name="INCR_COST" dataDxfId="0" dataCellStyle="Comma">
-      <calculatedColumnFormula>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</calculatedColumnFormula>
+      <calculatedColumnFormula>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2878,8 +2878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL773"/>
   <sheetViews>
-    <sheetView topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18214,8 +18214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA723D62-38EC-9448-8286-E86191556049}">
   <dimension ref="A1:AL773"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E56"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33549,8 +33549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677ECEB-A1A8-DC43-9E05-3CEFB316AC1E}">
   <dimension ref="A1:V773"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E56"/>
+    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42475,8 +42475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068950AB-F35C-0145-A678-27790CEEE3A1}">
   <dimension ref="A1:V773"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42642,12 +42642,12 @@
         <v>12803947954</v>
       </c>
       <c r="S3" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.3392949628521325</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.351929579873949</v>
       </c>
       <c r="T3" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.4171319191750236</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.3867184270950434</v>
       </c>
       <c r="U3"/>
       <c r="V3"/>
@@ -42708,12 +42708,12 @@
         <v>1008027542</v>
       </c>
       <c r="S4" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.1298039215686275</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1275566307455467</v>
       </c>
       <c r="T4" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.1384543517316121</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.1649744306431216</v>
       </c>
       <c r="U4"/>
       <c r="V4"/>
@@ -42774,12 +42774,12 @@
         <v>6254105024</v>
       </c>
       <c r="S5" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.000402057588837</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.0089066400399402</v>
       </c>
       <c r="T5" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0659496574243996</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0318982994109378</v>
       </c>
       <c r="U5"/>
       <c r="V5"/>
@@ -42840,12 +42840,12 @@
         <v>13326159383</v>
       </c>
       <c r="S6" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.0673699278068209</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.0764335332441646</v>
       </c>
       <c r="T6" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.1576185129106631</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.1065339062508848</v>
       </c>
       <c r="U6"/>
       <c r="V6"/>
@@ -42906,12 +42906,12 @@
         <v>1222705791</v>
       </c>
       <c r="S7" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.52813881374942273</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.54261986837981824</v>
       </c>
       <c r="T7" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.6005239253578607</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.56279611487786174</v>
       </c>
       <c r="U7"/>
       <c r="V7"/>
@@ -42972,12 +42972,12 @@
         <v>440831587</v>
       </c>
       <c r="S8" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.7414996878015554</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.76019777503090236</v>
       </c>
       <c r="T8" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.77142199161113045</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.76070064330185416</v>
       </c>
       <c r="U8"/>
       <c r="V8"/>
@@ -43038,12 +43038,12 @@
         <v>7176277816</v>
       </c>
       <c r="S9" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.93586741653354344</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.94381212535093706</v>
       </c>
       <c r="T9" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.99444350350331012</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.96425289332925979</v>
       </c>
       <c r="U9"/>
       <c r="V9"/>
@@ -43104,12 +43104,12 @@
         <v>17779605259</v>
       </c>
       <c r="S10" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.88284677613432305</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.90972521873249912</v>
       </c>
       <c r="T10" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.014588583380406</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.97287125037739397</v>
       </c>
       <c r="U10"/>
       <c r="V10"/>
@@ -43170,12 +43170,12 @@
         <v>23044994242</v>
       </c>
       <c r="S11" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.1598410266523063</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1654207561349086</v>
       </c>
       <c r="T11" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.2056853893907635</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.1922679591213283</v>
       </c>
       <c r="U11"/>
       <c r="V11"/>
@@ -43236,12 +43236,12 @@
         <v>3500861335</v>
       </c>
       <c r="S12" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.93769972734468898</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.93553833499285677</v>
       </c>
       <c r="T12" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.96217244461230655</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.9544183752705826</v>
       </c>
       <c r="U12"/>
       <c r="V12"/>
@@ -43302,12 +43302,12 @@
         <v>244077974</v>
       </c>
       <c r="S13" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.69890960253253609</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.70505789152955511</v>
       </c>
       <c r="T13" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.71509811364589337</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.70656350625583975</v>
       </c>
       <c r="U13"/>
       <c r="V13"/>
@@ -43368,12 +43368,12 @@
         <v>311197798</v>
       </c>
       <c r="S14" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.28203517587939708</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.30157618213660253</v>
       </c>
       <c r="T14" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.29469936367732452</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.28580907230578267</v>
       </c>
       <c r="U14"/>
       <c r="V14"/>
@@ -43434,12 +43434,12 @@
         <v>138744944</v>
       </c>
       <c r="S15" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.33454545454545448</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.33021582733812949</v>
       </c>
       <c r="T15" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.33707957016985923</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.33616692581384822</v>
       </c>
       <c r="U15"/>
       <c r="V15"/>
@@ -43500,12 +43500,12 @@
         <v>44154029243</v>
       </c>
       <c r="S16" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.41679503021480446</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.43541217470326243</v>
       </c>
       <c r="T16" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.48464425618982565</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.46131306910486858</v>
       </c>
       <c r="U16"/>
       <c r="V16"/>
@@ -43566,12 +43566,12 @@
         <v>130370471712</v>
       </c>
       <c r="S17" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.53702839353826248</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.56863109473387352</v>
       </c>
       <c r="T17" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.66867072417681661</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.61786480878739747</v>
       </c>
       <c r="U17"/>
       <c r="V17"/>
@@ -43632,12 +43632,12 @@
         <v>769167534</v>
       </c>
       <c r="S18" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.68420495447808594</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.69434021263289547</v>
       </c>
       <c r="T18" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.74883286659081594</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.72838600441614076</v>
       </c>
       <c r="U18"/>
       <c r="V18"/>
@@ -43698,12 +43698,12 @@
         <v>26758344631</v>
       </c>
       <c r="S19" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.79389511363914966</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.78263540895028116</v>
       </c>
       <c r="T19" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.80310524775631875</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.79896803154866891</v>
       </c>
       <c r="U19"/>
       <c r="V19"/>
@@ -43764,12 +43764,12 @@
         <v>521842133</v>
       </c>
       <c r="S20" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.7226749942874553</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.72220575155647793</v>
       </c>
       <c r="T20" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.72964941548029949</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.72733144271240513</v>
       </c>
       <c r="U20"/>
       <c r="V20"/>
@@ -43830,12 +43830,12 @@
         <v>49831568367</v>
       </c>
       <c r="S21" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.65837836720242104</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.67205342491245279</v>
       </c>
       <c r="T21" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.71664604897697015</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.70438295061708467</v>
       </c>
       <c r="U21"/>
       <c r="V21"/>
@@ -43896,12 +43896,12 @@
         <v>3531501172</v>
       </c>
       <c r="S22" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.97489991528098474</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.98385434558570939</v>
       </c>
       <c r="T22" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0539326989743958</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0226972884426768</v>
       </c>
       <c r="U22"/>
       <c r="V22"/>
@@ -43962,12 +43962,12 @@
         <v>1151641873</v>
       </c>
       <c r="S23" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.0072472981563889</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.0124330858228285</v>
       </c>
       <c r="T23" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0860183308110796</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0426486859907356</v>
       </c>
       <c r="U23"/>
       <c r="V23"/>
@@ -44028,12 +44028,12 @@
         <v>630253931</v>
       </c>
       <c r="S24" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.8061178075960882</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.81364296081277221</v>
       </c>
       <c r="T24" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.84708404689785577</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.8234166399969236</v>
       </c>
       <c r="U24"/>
       <c r="V24"/>
@@ -44094,12 +44094,12 @@
         <v>2314975801</v>
       </c>
       <c r="S25" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.0135486171242296</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.016281914080416</v>
       </c>
       <c r="T25" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0377420083116133</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0312864545968981</v>
       </c>
       <c r="U25"/>
       <c r="V25"/>
@@ -44160,12 +44160,12 @@
         <v>5529634198</v>
       </c>
       <c r="S26" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.68988829595566159</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.70479866203525021</v>
       </c>
       <c r="T26" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.7963199566139032</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.74338967417944724</v>
       </c>
       <c r="U26"/>
       <c r="V26"/>
@@ -44226,12 +44226,12 @@
         <v>1495130786</v>
       </c>
       <c r="S27" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.84527703688792721</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.85034871019242075</v>
       </c>
       <c r="T27" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.88154250949892954</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.86652375347319066</v>
       </c>
       <c r="U27"/>
       <c r="V27"/>
@@ -44292,12 +44292,12 @@
         <v>5233718683</v>
       </c>
       <c r="S28" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.28135741804507819</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.28984839897988102</v>
       </c>
       <c r="T28" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.31410771357388523</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.30318529215205414</v>
       </c>
       <c r="U28"/>
       <c r="V28"/>
@@ -44358,12 +44358,12 @@
         <v>269262714</v>
       </c>
       <c r="S29" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.28358564787221363</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.29826933477555428</v>
       </c>
       <c r="T29" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.32779407210518241</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.30882247455452094</v>
       </c>
       <c r="U29"/>
       <c r="V29"/>
@@ -44424,12 +44424,12 @@
         <v>16888573385</v>
       </c>
       <c r="S30" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.31557548080935738</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.33172863558066235</v>
       </c>
       <c r="T30" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.37899205011162329</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.35501330303773004</v>
       </c>
       <c r="U30"/>
       <c r="V30"/>
@@ -44490,12 +44490,12 @@
         <v>15439866615</v>
       </c>
       <c r="S31" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.95002396081076279</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.94908352266163498</v>
       </c>
       <c r="T31" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.99797930080010877</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.98182997846431763</v>
       </c>
       <c r="U31"/>
       <c r="V31"/>
@@ -44556,12 +44556,12 @@
         <v>2262081369</v>
       </c>
       <c r="S32" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.1441885964912282</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1470541017819875</v>
       </c>
       <c r="T32" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.180923894971488</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.1651546403585735</v>
       </c>
       <c r="U32"/>
       <c r="V32"/>
@@ -44622,12 +44622,12 @@
         <v>12058538684</v>
       </c>
       <c r="S33" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.054133001417358</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.0861585114447978</v>
       </c>
       <c r="T33" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.1899826786186849</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.1297069004382858</v>
       </c>
       <c r="U33"/>
       <c r="V33"/>
@@ -44688,12 +44688,12 @@
         <v>1916476339</v>
       </c>
       <c r="S34" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.9307000234121543</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.94248303283745805</v>
       </c>
       <c r="T34" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0064389603813377</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.96356284302017037</v>
       </c>
       <c r="U34"/>
       <c r="V34"/>
@@ -44754,12 +44754,12 @@
         <v>669836653</v>
       </c>
       <c r="S35" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>5.1715522984676854E-2</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>5.7299451918285893E-2</v>
       </c>
       <c r="T35" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>7.0781880228006022E-2</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>6.0567131227337256E-2</v>
       </c>
       <c r="U35"/>
       <c r="V35"/>
@@ -44820,12 +44820,12 @@
         <v>2595484867</v>
       </c>
       <c r="S36" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.98912731210359994</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.99405308969021999</v>
       </c>
       <c r="T36" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0168021746896394</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0180419813104744</v>
       </c>
       <c r="U36"/>
       <c r="V36"/>
@@ -44886,12 +44886,12 @@
         <v>2085055032</v>
       </c>
       <c r="S37" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.54750755734692658</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.60482271753787575</v>
       </c>
       <c r="T37" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.75049060427536163</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.64404348959797386</v>
       </c>
       <c r="U37"/>
       <c r="V37"/>
@@ -44952,12 +44952,12 @@
         <v>5570641313</v>
       </c>
       <c r="S38" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.7035261095842347</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.7118704569055034</v>
       </c>
       <c r="T38" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.7678588180511841</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.733385148293197</v>
       </c>
       <c r="U38"/>
       <c r="V38"/>
@@ -45018,12 +45018,12 @@
         <v>73587025829</v>
       </c>
       <c r="S39" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.93140894903210114</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.94681224698539057</v>
       </c>
       <c r="T39" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0074574249939663</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.99625739019586912</v>
       </c>
       <c r="U39"/>
       <c r="V39"/>
@@ -45084,12 +45084,12 @@
         <v>2584644313</v>
       </c>
       <c r="S40" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.76704252505099868</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.76798434016638573</v>
       </c>
       <c r="T40" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.79202436417392086</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.77369316156482171</v>
       </c>
       <c r="U40"/>
       <c r="V40"/>
@@ -45150,12 +45150,12 @@
         <v>14982934052</v>
       </c>
       <c r="S41" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.85401799141443147</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.85364882495467564</v>
       </c>
       <c r="T41" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.89519810764700058</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.88140874518237955</v>
       </c>
       <c r="U41"/>
       <c r="V41"/>
@@ -45216,12 +45216,12 @@
         <v>5050482876</v>
       </c>
       <c r="S42" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.96022225217534563</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.99026949464149583</v>
       </c>
       <c r="T42" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0881861727059428</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0305447089437076</v>
       </c>
       <c r="U42"/>
       <c r="V42"/>
@@ -45282,12 +45282,12 @@
         <v>1453400407</v>
       </c>
       <c r="S43" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.6092518388923378</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.61714417744916816</v>
       </c>
       <c r="T43" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.66378372568448007</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.63172317643310083</v>
       </c>
       <c r="U43"/>
       <c r="V43"/>
@@ -45348,12 +45348,12 @@
         <v>885669697</v>
       </c>
       <c r="S44" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.186788323875227</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1890027958993477</v>
       </c>
       <c r="T44" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.2483922454444007</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.2193395833815028</v>
       </c>
       <c r="U44"/>
       <c r="V44"/>
@@ -45414,12 +45414,12 @@
         <v>5107076723</v>
       </c>
       <c r="S45" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.78701986155725456</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.78702896119870291</v>
       </c>
       <c r="T45" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.82278232085671954</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.81024851344231896</v>
       </c>
       <c r="U45"/>
       <c r="V45"/>
@@ -45480,12 +45480,12 @@
         <v>60607198</v>
       </c>
       <c r="S46" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.79712918660287091</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.84782608695652173</v>
       </c>
       <c r="T46" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.81866478996749659</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.81230586558784879</v>
       </c>
       <c r="U46"/>
       <c r="V46"/>
@@ -45546,12 +45546,12 @@
         <v>496022304</v>
       </c>
       <c r="S47" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.46078280890253254</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.47464746474647468</v>
       </c>
       <c r="T47" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.49886652503105844</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.48239425170572869</v>
       </c>
       <c r="U47"/>
       <c r="V47"/>
@@ -45612,12 +45612,12 @@
         <v>82551469</v>
       </c>
       <c r="S48" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.21118530884808018</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.33029612756264237</v>
       </c>
       <c r="T48" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.17914311709528685</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.17561697573806145</v>
       </c>
       <c r="U48"/>
       <c r="V48"/>
@@ -45678,12 +45678,12 @@
         <v>808788311</v>
       </c>
       <c r="S49" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.0623283459725354</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1170544055687857</v>
       </c>
       <c r="T49" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.1644042034786253</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.1293327740155936</v>
       </c>
       <c r="U49"/>
       <c r="V49"/>
@@ -45744,12 +45744,12 @@
         <v>2653294315</v>
       </c>
       <c r="S50" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.85219998065951064</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.858844777881977</v>
       </c>
       <c r="T50" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.91637544907482704</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.8829104767880529</v>
       </c>
       <c r="U50"/>
       <c r="V50"/>
@@ -45810,12 +45810,12 @@
         <v>12037920155</v>
       </c>
       <c r="S51" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.23027805362462761</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.24216821143805389</v>
       </c>
       <c r="T51" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.27426108948476258</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.25885565889308326</v>
       </c>
       <c r="U51"/>
       <c r="V51"/>
@@ -45876,12 +45876,12 @@
         <v>21148557298</v>
       </c>
       <c r="S52" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.1231597004354512</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1611411780330698</v>
       </c>
       <c r="T52" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.3077828925442545</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.224820258088354</v>
       </c>
       <c r="U52"/>
       <c r="V52"/>
@@ -45942,12 +45942,12 @@
         <v>13355444162</v>
       </c>
       <c r="S53" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.92942794863625089</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.95629702014434237</v>
       </c>
       <c r="T53" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.0865702570148899</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.0195980970432594</v>
       </c>
       <c r="U53"/>
       <c r="V53"/>
@@ -46008,12 +46008,12 @@
         <v>63547962580</v>
       </c>
       <c r="S54" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.32913167019239187</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.34194933235041769</v>
       </c>
       <c r="T54" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.38765229327771733</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.36078248268322688</v>
       </c>
       <c r="U54"/>
       <c r="V54"/>
@@ -46074,12 +46074,12 @@
         <v>7620354891</v>
       </c>
       <c r="S55" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>1.1094557990642699</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>1.1258096497025778</v>
       </c>
       <c r="T55" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>1.2044062812918859</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>1.156123752154171</v>
       </c>
       <c r="U55"/>
       <c r="V55"/>
@@ -46140,12 +46140,12 @@
         <v>3335548857</v>
       </c>
       <c r="S56" s="1">
-        <f>(Table134[[#This Row],[2050_BUILDINGS]]/Table134[[#This Row],[2020_BUILDINGS]])-1</f>
-        <v>0.59625523336951458</v>
+        <f>(Table1345[[#This Row],[2050_BUILDINGS]]/Table1345[[#This Row],[2020_BUILDINGS]])-1</f>
+        <v>0.60353420933393753</v>
       </c>
       <c r="T56" s="1">
-        <f>(Table134[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table134[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
-        <v>0.65168733853160865</v>
+        <f>(Table1345[[#This Row],[2050_TOTAL_REPL_COST_USD]]/Table1345[[#This Row],[2020_TOTAL_REPL_COST_USD]])-1</f>
+        <v>0.62837023404390258</v>
       </c>
       <c r="U56"/>
       <c r="V56"/>

</xml_diff>